<commit_message>
Mise à jour des fichiers templates
Upload des dernières versions des fichiers templates :
- Prices inputs
- User inputs
(mêmes fichiers sur le SharePoint)
</commit_message>
<xml_diff>
--- a/Templates/User_inputs.xlsx
+++ b/Templates/User_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.perreyon\Documents\ECL cost models\ecl_cost_models\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://supergridinstitute.sharepoint.com/sites/CostmodelsforgridTEA/Documents partages/Projet Option Energie ECL/2. Base De Données/4. Hypothèses de prix Utilisateurs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEAA5D6-2695-42C9-B786-2105A6BAF728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0548D9B-54AC-4C66-A4F4-F859083FD76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3D3606FB-9301-4AD0-98C2-CCA38780FF77}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{3D3606FB-9301-4AD0-98C2-CCA38780FF77}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustering" sheetId="5" r:id="rId1"/>
@@ -134,6 +134,9 @@
     <t>Node</t>
   </si>
   <si>
+    <t>Country names</t>
+  </si>
+  <si>
     <t>AL</t>
   </si>
   <si>
@@ -584,25 +587,14 @@
   </si>
   <si>
     <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>Country names</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -706,25 +698,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -733,15 +722,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,48 +815,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -935,6 +885,48 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -954,14 +946,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C5153C5-1D61-42E7-BE5A-CC979AA97894}" name="Zone_clustering" displayName="Zone_clustering" ref="A1:B11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C5153C5-1D61-42E7-BE5A-CC979AA97894}" name="Zone_clustering" displayName="Zone_clustering" ref="A1:B11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A1:B11" xr:uid="{5C5153C5-1D61-42E7-BE5A-CC979AA97894}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7560A568-94AC-4E07-91A0-66A52F360C1C}" name="Zone" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{8166EBCB-E17C-4D34-829A-C2D67CF8AE0E}" name="Zone name" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{7560A568-94AC-4E07-91A0-66A52F360C1C}" name="Zone" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{8166EBCB-E17C-4D34-829A-C2D67CF8AE0E}" name="Zone name" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1305,130 +1297,130 @@
       <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.90625" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="11"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1448,26 +1440,26 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1476,9 +1468,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="str">
         <f>VLOOKUP(A2,BDD!B:D,3,FALSE)</f>
@@ -1492,9 +1484,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="str">
         <f>VLOOKUP(A3,BDD!B:D,3,FALSE)</f>
@@ -1508,9 +1500,9 @@
         <v>Central Europe</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP(A4,BDD!B:D,3,FALSE)</f>
@@ -1524,9 +1516,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(A5,BDD!B:D,3,FALSE)</f>
@@ -1540,9 +1532,9 @@
         <v>Benelux</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(A6,BDD!B:D,3,FALSE)</f>
@@ -1556,9 +1548,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(A7,BDD!B:D,3,FALSE)</f>
@@ -1572,9 +1564,9 @@
         <v>Italy</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(A8,BDD!B:D,3,FALSE)</f>
@@ -1588,9 +1580,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(A9,BDD!B:D,3,FALSE)</f>
@@ -1604,9 +1596,9 @@
         <v>Central Europe</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(A10,BDD!B:D,3,FALSE)</f>
@@ -1620,9 +1612,9 @@
         <v>Germany</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(A11,BDD!B:D,3,FALSE)</f>
@@ -1636,9 +1628,9 @@
         <v>Scandinavia</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(A12,BDD!B:D,3,FALSE)</f>
@@ -1652,9 +1644,9 @@
         <v>Estern Europe</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(A13,BDD!B:D,3,FALSE)</f>
@@ -1668,9 +1660,9 @@
         <v>Iberian</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP(A14,BDD!B:D,3,FALSE)</f>
@@ -1684,9 +1676,9 @@
         <v>Scandinavia</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP(A15,BDD!B:D,3,FALSE)</f>
@@ -1700,9 +1692,9 @@
         <v>France</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" t="str">
         <f>VLOOKUP(A16,BDD!B:D,3,FALSE)</f>
@@ -1716,9 +1708,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(A17,BDD!B:D,3,FALSE)</f>
@@ -1732,9 +1724,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(A18,BDD!B:D,3,FALSE)</f>
@@ -1748,9 +1740,9 @@
         <v>Central Europe</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(A19,BDD!B:D,3,FALSE)</f>
@@ -1764,9 +1756,9 @@
         <v>British</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(A20,BDD!B:D,3,FALSE)</f>
@@ -1780,9 +1772,9 @@
         <v>Italy</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(A21,BDD!B:D,3,FALSE)</f>
@@ -1796,9 +1788,9 @@
         <v>Estern Europe</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(A22,BDD!B:D,3,FALSE)</f>
@@ -1812,9 +1804,9 @@
         <v>Benelux</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(A23,BDD!B:D,3,FALSE)</f>
@@ -1828,9 +1820,9 @@
         <v>Estern Europe</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP(A24,BDD!B:D,3,FALSE)</f>
@@ -1844,9 +1836,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP(A25,BDD!B:D,3,FALSE)</f>
@@ -1860,9 +1852,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP(A26,BDD!B:D,3,FALSE)</f>
@@ -1876,9 +1868,9 @@
         <v>Italy</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" t="str">
         <f>VLOOKUP(A27,BDD!B:D,3,FALSE)</f>
@@ -1892,9 +1884,9 @@
         <v>Benelux</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP(A28,BDD!B:D,3,FALSE)</f>
@@ -1908,9 +1900,9 @@
         <v>Scandinavia</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" t="str">
         <f>VLOOKUP(A29,BDD!B:D,3,FALSE)</f>
@@ -1924,9 +1916,9 @@
         <v>Estern Europe</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B30" t="str">
         <f>VLOOKUP(A30,BDD!B:D,3,FALSE)</f>
@@ -1940,9 +1932,9 @@
         <v>Iberian</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B31" t="str">
         <f>VLOOKUP(A31,BDD!B:D,3,FALSE)</f>
@@ -1956,9 +1948,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B32" t="str">
         <f>VLOOKUP(A32,BDD!B:D,3,FALSE)</f>
@@ -1972,9 +1964,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B33" t="str">
         <f>VLOOKUP(A33,BDD!B:D,3,FALSE)</f>
@@ -1988,9 +1980,9 @@
         <v>Scandinavia</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B34" t="str">
         <f>VLOOKUP(A34,BDD!B:D,3,FALSE)</f>
@@ -2004,9 +1996,9 @@
         <v>Balkans</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B35" t="str">
         <f>VLOOKUP(A35,BDD!B:D,3,FALSE)</f>
@@ -2020,9 +2012,9 @@
         <v>Central Europe</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B36" t="str">
         <f>VLOOKUP(A36,BDD!B:D,3,FALSE)</f>
@@ -2067,155 +2059,155 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
@@ -2244,25 +2236,25 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B2">
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2017</v>
       </c>
@@ -2286,115 +2278,115 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.6328125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.08984375" style="2"/>
+    <col min="1" max="1" width="6.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5703125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>88</v>
       </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
         <v>90</v>
       </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
         <v>92</v>
       </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="8" t="s">
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>96</v>
       </c>
+    </row>
+    <row r="7" spans="1:2" ht="30">
+      <c r="A7" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
         <v>98</v>
       </c>
+    </row>
+    <row r="8" spans="1:2" ht="30">
+      <c r="A8" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="B8" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="8" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>102</v>
       </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
         <v>104</v>
       </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="B11" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="8" t="s">
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>108</v>
       </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2409,520 +2401,520 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.08984375" style="4"/>
-    <col min="4" max="4" width="22" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="22" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="17" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+      <c r="D1" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+      <c r="D2" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4">
         <v>40</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
+      <c r="D3" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4">
         <v>56</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
+      <c r="A5" s="4">
+        <v>70</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>70</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+      <c r="D5" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4">
         <v>100</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+      <c r="D6" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4">
         <v>191</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4">
+        <v>196</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4">
+        <v>203</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="4">
+        <v>208</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4">
+        <v>233</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4">
+        <v>246</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4">
+        <v>250</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="4">
+        <v>276</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="4">
+        <v>300</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
-        <v>196</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4">
+        <v>348</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <v>372</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4">
+        <v>380</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4">
+        <v>428</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4">
+        <v>440</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="4">
+        <v>442</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4">
+        <v>470</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="4">
+        <v>499</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="4">
+        <v>528</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="4">
+        <v>807</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="4">
+        <v>578</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="4">
+        <v>616</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="4">
+        <v>620</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4">
+        <v>642</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="4">
+        <v>688</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="4">
+        <v>703</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="4">
+        <v>705</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="4">
+        <v>724</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="4">
+        <v>752</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4">
+        <v>756</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
-        <v>203</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="5">
-        <v>208</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>233</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
-        <v>246</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
-        <v>250</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
-        <v>276</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
-        <v>300</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
-        <v>348</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
-        <v>372</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="5">
-        <v>380</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="5">
-        <v>428</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="5">
-        <v>440</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="5">
-        <v>442</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="5">
-        <v>470</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="5">
-        <v>499</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="5">
-        <v>528</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="5">
-        <v>807</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="5">
-        <v>578</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="5">
-        <v>616</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="5">
-        <v>620</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="5">
-        <v>642</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="5">
-        <v>688</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="5">
-        <v>703</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="5">
-        <v>705</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="5">
-        <v>724</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="5">
-        <v>752</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="5">
-        <v>756</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="5">
+      <c r="D35" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="4">
         <v>826</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="B36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>178</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2931,9 +2923,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037B722CC9AC5C444AAE886EDD40B6781" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2d811b84d58eb5860d404ba8595f6c98">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="780399fe-2133-4349-a0e7-53824f1dae47" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2abf1b2d58055100e5d460db1a46c346" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037B722CC9AC5C444AAE886EDD40B6781" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="62f3e12650e25baa9087e793e2ad5c2b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="780399fe-2133-4349-a0e7-53824f1dae47" xmlns:ns3="27d3a517-4705-4b45-9ea7-12bdf953c8a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6321ff521e5dc27e65c92a6ebe88ef1a" ns2:_="" ns3:_="">
     <xsd:import namespace="780399fe-2133-4349-a0e7-53824f1dae47"/>
+    <xsd:import namespace="27d3a517-4705-4b45-9ea7-12bdf953c8a9"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -2944,6 +2937,12 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2973,6 +2972,50 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="4b932911-d067-401a-a54e-ba3cc5b14725" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="27d3a517-4705-4b45-9ea7-12bdf953c8a9" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{a70856a4-270c-4974-9c66-39df1b9929e9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="27d3a517-4705-4b45-9ea7-12bdf953c8a9">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -3076,7 +3119,12 @@
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="780399fe-2133-4349-a0e7-53824f1dae47">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="27d3a517-4705-4b45-9ea7-12bdf953c8a9" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -3090,36 +3138,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5511451E-3EAD-4C47-B52B-71C36F7E14BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="780399fe-2133-4349-a0e7-53824f1dae47"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAF17669-6C7C-4E21-8494-284FAAABAA3B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{095D11A8-AEE4-4713-9C10-8A612E26E3A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{095D11A8-AEE4-4713-9C10-8A612E26E3A0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AF68339-774A-4120-A9CD-FEEF8F07C651}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AF68339-774A-4120-A9CD-FEEF8F07C651}"/>
 </file>
</xml_diff>